<commit_message>
Removed offset in python code, fixed reported height, tested full range for Warrior's data, 15 Hz was the only valid frequency for amplitud range
</commit_message>
<xml_diff>
--- a/Datasets/II Semester 2025/Results - Manuales excel.xlsx
+++ b/Datasets/II Semester 2025/Results - Manuales excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eWave\eWave\Datasets\II Semester 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AE06B6D1-F527-42DC-B8EE-1D60F79B5053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724C0DD2-7EC5-4CA6-84F3-A87F342BF9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="Pruebas Olas Guerrero" sheetId="2" r:id="rId2"/>
     <sheet name="Olas Guerrero Final" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
   <si>
     <t>Pos</t>
   </si>
@@ -66,9 +79,6 @@
     <t>Variador(Hz)</t>
   </si>
   <si>
-    <t>Ola (Hz)</t>
-  </si>
-  <si>
     <t>Para 15 Hz</t>
   </si>
   <si>
@@ -94,6 +104,45 @@
   </si>
   <si>
     <t>Agua mayor</t>
+  </si>
+  <si>
+    <t>Ola (s)</t>
+  </si>
+  <si>
+    <t>Amplitud (mm)</t>
+  </si>
+  <si>
+    <t>Frecuencia (Hz)</t>
+  </si>
+  <si>
+    <t>Brazo Máximo (mm)</t>
+  </si>
+  <si>
+    <t>Brazo Mínimo (mm)</t>
+  </si>
+  <si>
+    <t>Con nuevo nivel de agua</t>
+  </si>
+  <si>
+    <t>11.65 (Periodo 3.598 s)</t>
+  </si>
+  <si>
+    <t>15 (Periodo 2.68 s)</t>
+  </si>
+  <si>
+    <t>13.325 (Periodo 3.104 s)</t>
+  </si>
+  <si>
+    <t>14.1625 (Periodo 2.945 s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barrido a 15 Hz </t>
+  </si>
+  <si>
+    <t>Periodo(s)</t>
+  </si>
+  <si>
+    <t>Pruebas realizadas con sensores</t>
   </si>
 </sst>
 </file>
@@ -424,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -550,6 +599,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -595,7 +677,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,6 +686,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2174,6 +2286,750 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Frecuencia vs Amplitud Bond (Brazo 90 mm)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Results - Manuales'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Results - Manuales'!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2CF-4F7E-BA98-673D458A68A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="609823279"/>
+        <c:axId val="609817999"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="609823279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609817999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="609817999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609823279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Pruebas Olas Guerrero'!$K$18:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Pruebas Olas Guerrero'!$L$18:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-872E-4080-974E-F929E4E0A8E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="609821359"/>
+        <c:axId val="609821839"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="609821359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="110"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609821839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="609821839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609821359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2334,6 +3190,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3883,6 +4819,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4539,6 +6507,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A8E5E69-BD52-35FA-EBA0-AE4F1DD16724}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>336613</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>48827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>62885</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>17755</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BED7B06-7ED8-EECE-C379-EE6A41331286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4866,7 +6911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AC0B2E-32D4-4C37-A5A1-F9A5D8F7C8EA}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView topLeftCell="D18" workbookViewId="0"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4909,13 +6956,13 @@
         <v>2.6989999999999998</v>
       </c>
       <c r="P2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" t="s">
         <v>18</v>
-      </c>
-      <c r="V2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -4935,22 +6982,22 @@
         <v>2.5150000000000001</v>
       </c>
       <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
       <c r="S3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" t="s">
-        <v>17</v>
-      </c>
       <c r="V3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" t="s">
         <v>16</v>
-      </c>
-      <c r="W3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -5415,7 +7462,7 @@
         <v>12</v>
       </c>
       <c r="S26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -5438,13 +7485,13 @@
         <v>13</v>
       </c>
       <c r="Q27" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="S27" t="s">
         <v>13</v>
       </c>
       <c r="T27" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -6001,64 +8048,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC90928-3868-4917-A345-B6867C183697}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I12" zoomScale="103" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="O2" s="1">
+        <v>155</v>
+      </c>
+      <c r="P2" s="1">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1">
         <v>15</v>
       </c>
       <c r="D3" s="1">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1">
-        <v>2.6890000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1">
+        <v>170</v>
+      </c>
+      <c r="P3" s="1">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2.6829999999999998</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1">
         <v>15</v>
@@ -6070,137 +8151,812 @@
         <v>2.6890000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
+        <v>125</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>125</v>
+      </c>
+      <c r="C7" s="1">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.6890000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
         <v>120</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>15</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D8" s="1">
         <v>51</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E8" s="1">
         <v>2.6829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="K9" s="7"/>
+      <c r="L9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
         <v>140</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C10" s="1">
         <v>13</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D10" s="1">
         <v>21</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E10" s="1">
         <v>3.0790000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+      <c r="K10" s="7"/>
+      <c r="L10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8">
+        <f>11.65+AA11</f>
+        <v>12.487500000000001</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="8"/>
+      <c r="V10" s="4"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="AA10" s="1">
+        <f>15-11.65</f>
+        <v>3.3499999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
         <v>200</v>
-      </c>
-      <c r="C9" s="1">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3.1059999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>230</v>
-      </c>
-      <c r="C10" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3.0219999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
-        <v>230</v>
       </c>
       <c r="C11" s="1">
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1">
-        <v>3.11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+        <v>3.1059999999999999</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA11" s="1">
+        <f>AA10/4</f>
+        <v>0.83749999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
+        <v>230</v>
+      </c>
+      <c r="C12" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.0219999999999998</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="7">
+        <v>270</v>
+      </c>
+      <c r="M12" s="7">
+        <v>49</v>
+      </c>
+      <c r="N12" s="7">
         <v>290</v>
       </c>
-      <c r="C12" s="1">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1">
-        <v>3.1859999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="O12" s="7">
+        <v>49</v>
+      </c>
+      <c r="P12" s="7">
+        <v>290</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>50</v>
+      </c>
+      <c r="R12" s="7">
+        <v>210</v>
+      </c>
+      <c r="S12" s="7">
+        <v>52</v>
+      </c>
+      <c r="T12" s="7">
+        <v>120</v>
+      </c>
+      <c r="U12" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
-        <v>290</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1">
         <v>13</v>
       </c>
       <c r="D13" s="1">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="7">
+        <v>310</v>
+      </c>
+      <c r="M13" s="7">
+        <v>62</v>
+      </c>
+      <c r="N13" s="7">
+        <v>310</v>
+      </c>
+      <c r="O13" s="7">
         <v>52</v>
       </c>
-      <c r="E13" s="1">
+      <c r="P13" s="7">
+        <v>310</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>56</v>
+      </c>
+      <c r="R13" s="7">
+        <v>300</v>
+      </c>
+      <c r="S13" s="7">
+        <v>74</v>
+      </c>
+      <c r="T13" s="7">
+        <v>180</v>
+      </c>
+      <c r="U13" s="7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>270</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3.8039999999999998</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>270</v>
+      </c>
+      <c r="C15" s="1">
+        <v>11.23</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3.7480000000000002</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>270</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3.6320000000000001</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>270</v>
+      </c>
+      <c r="C17" s="1">
+        <v>11.65</v>
+      </c>
+      <c r="D17" s="1">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.5979999999999999</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>270</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11.75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3.5640000000000001</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="10">
+        <v>120</v>
+      </c>
+      <c r="L18" s="10">
+        <v>51</v>
+      </c>
+      <c r="M18" s="13">
+        <v>2.6880000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>270</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="1">
+        <v>130</v>
+      </c>
+      <c r="L19" s="1">
+        <v>53</v>
+      </c>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>270</v>
+      </c>
+      <c r="C20" s="1">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.1619999999999999</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1">
+        <v>140</v>
+      </c>
+      <c r="L20" s="1">
+        <v>56</v>
+      </c>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>290</v>
+      </c>
+      <c r="C21" s="1">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="K21" s="1">
+        <v>150</v>
+      </c>
+      <c r="L21" s="1">
+        <v>62</v>
+      </c>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>290</v>
+      </c>
+      <c r="C22" s="1">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1">
         <v>3.21</v>
       </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
-        <v>155</v>
-      </c>
-      <c r="C18" s="1">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="1">
+        <v>160</v>
+      </c>
+      <c r="L22" s="1">
+        <v>64</v>
+      </c>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>290</v>
+      </c>
+      <c r="C23" s="1">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.972</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="10">
         <v>170</v>
       </c>
-      <c r="C19" s="1">
-        <v>11.2</v>
+      <c r="L23" s="10">
+        <v>68</v>
+      </c>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>290</v>
+      </c>
+      <c r="C24" s="1">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <v>92</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.5019999999999998</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="12">
+        <v>180</v>
+      </c>
+      <c r="L24" s="12">
+        <v>74</v>
+      </c>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>310</v>
+      </c>
+      <c r="C25" s="1">
+        <v>11.65</v>
+      </c>
+      <c r="D25" s="1">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3.7719999999999998</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="6"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="K27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="10">
+        <v>120</v>
+      </c>
+      <c r="L28" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>110</v>
+      </c>
+      <c r="C29" s="1">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1">
+        <v>47</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="K29" s="1">
+        <v>135</v>
+      </c>
+      <c r="L29" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>120</v>
+      </c>
+      <c r="C30" s="1">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1">
+        <v>51</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2.6829999999999998</v>
+      </c>
+      <c r="K30" s="1">
+        <v>145</v>
+      </c>
+      <c r="L30" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>120</v>
+      </c>
+      <c r="C31" s="1">
+        <v>13.01</v>
+      </c>
+      <c r="D31" s="1">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="K31" s="1">
+        <v>164</v>
+      </c>
+      <c r="L31" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>180</v>
+      </c>
+      <c r="C32" s="1">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1">
+        <v>74</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.6989999999999998</v>
+      </c>
+      <c r="K32" s="1">
+        <v>172</v>
+      </c>
+      <c r="L32" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>270</v>
+      </c>
+      <c r="C33" s="1">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1">
+        <v>51</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3.8039999999999998</v>
+      </c>
+      <c r="K33" s="12">
+        <v>180</v>
+      </c>
+      <c r="L33" s="12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>270</v>
+      </c>
+      <c r="C34" s="1">
+        <v>11.23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3.7480000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>270</v>
+      </c>
+      <c r="C35" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.6320000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>270</v>
+      </c>
+      <c r="C36" s="1">
+        <v>11.65</v>
+      </c>
+      <c r="D36" s="1">
+        <v>49</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.5979999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>270</v>
+      </c>
+      <c r="C37" s="1">
+        <v>11.75</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3.5640000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>270</v>
+      </c>
+      <c r="C38" s="1">
+        <v>12</v>
+      </c>
+      <c r="D38" s="1">
+        <v>38</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3.4510000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>270</v>
+      </c>
+      <c r="C39" s="1">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3.1619999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>290</v>
+      </c>
+      <c r="C40" s="1">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1">
+        <v>52</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>290</v>
+      </c>
+      <c r="C41" s="1">
+        <v>14</v>
+      </c>
+      <c r="D41" s="1">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2.972</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>290</v>
+      </c>
+      <c r="C42" s="1">
+        <v>15</v>
+      </c>
+      <c r="D42" s="1">
+        <v>92</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2.5019999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="12">
+        <v>310</v>
+      </c>
+      <c r="C43" s="12">
+        <v>11.65</v>
+      </c>
+      <c r="D43" s="12">
+        <v>62</v>
+      </c>
+      <c r="E43" s="12">
+        <v>3.7719999999999998</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="L9:U9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="M18:M24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6221,16 +8977,16 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Did some crazy stuff, got rolling avgs but not enough raw data available
</commit_message>
<xml_diff>
--- a/Datasets/II Semester 2025/Results - Manuales excel.xlsx
+++ b/Datasets/II Semester 2025/Results - Manuales excel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eWave\eWave\Datasets\II Semester 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724C0DD2-7EC5-4CA6-84F3-A87F342BF9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D630434-A787-452C-B753-0E49D76C3E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
   </bookViews>
   <sheets>
     <sheet name="Results - Manuales" sheetId="1" r:id="rId1"/>
     <sheet name="Pruebas Olas Guerrero" sheetId="2" r:id="rId2"/>
     <sheet name="Olas Guerrero Final" sheetId="3" r:id="rId3"/>
+    <sheet name="Validation Media Movil" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
   <si>
     <t>Pos</t>
   </si>
@@ -136,20 +137,71 @@
     <t>14.1625 (Periodo 2.945 s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Barrido a 15 Hz </t>
-  </si>
-  <si>
     <t>Periodo(s)</t>
   </si>
   <si>
     <t>Pruebas realizadas con sensores</t>
+  </si>
+  <si>
+    <t>Barrido a 15 Hz Solo manuales</t>
+  </si>
+  <si>
+    <t>PP (mm)</t>
+  </si>
+  <si>
+    <t>PP manual (mm)</t>
+  </si>
+  <si>
+    <t>Pruebas a 15 Hz</t>
+  </si>
+  <si>
+    <t>Pruebas a 11.65 Hz</t>
+  </si>
+  <si>
+    <t>Rangos máximos y mínimos medidos manualmente</t>
+  </si>
+  <si>
+    <t>Con sensores</t>
+  </si>
+  <si>
+    <t>Pruebas a 12.49 Hz</t>
+  </si>
+  <si>
+    <t>Pruebas a 13.33 Hz</t>
+  </si>
+  <si>
+    <t>Pruebas a 14.16 Hz</t>
+  </si>
+  <si>
+    <t>Brazo</t>
+  </si>
+  <si>
+    <t>Medidas con sensores</t>
+  </si>
+  <si>
+    <t>Datos manuales</t>
+  </si>
+  <si>
+    <t>15 Hz</t>
+  </si>
+  <si>
+    <t>Datos Sin Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos con 3 puntos </t>
+  </si>
+  <si>
+    <t>Datos con 4 puntos</t>
+  </si>
+  <si>
+    <t>Datos con 5 puntos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +339,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -632,6 +691,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -677,7 +762,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,31 +776,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6911,9 +7014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AC0B2E-32D4-4C37-A5A1-F9A5D8F7C8EA}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8050,8 +8151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC90928-3868-4917-A345-B6867C183697}">
   <dimension ref="B2:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I12" zoomScale="103" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView topLeftCell="A22" zoomScale="103" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8194,19 +8295,19 @@
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="K9" s="7"/>
-      <c r="L9" s="8" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
@@ -8221,31 +8322,31 @@
       <c r="E10" s="1">
         <v>3.0790000000000002</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="6"/>
+      <c r="L10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9">
         <f>11.65+AA11</f>
         <v>12.487500000000001</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8" t="s">
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8" t="s">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8" t="s">
+      <c r="S10" s="9"/>
+      <c r="T10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="U10" s="8"/>
+      <c r="U10" s="9"/>
       <c r="V10" s="4"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
       <c r="AA10" s="1">
         <f>15-11.65</f>
         <v>3.3499999999999996</v>
@@ -8264,35 +8365,35 @@
       <c r="E11" s="1">
         <v>3.1059999999999999</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7" t="s">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="U11" s="7" t="s">
+      <c r="U11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AA11" s="1">
@@ -8313,37 +8414,37 @@
       <c r="E12" s="1">
         <v>3.0219999999999998</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>270</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>49</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <v>290</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="6">
         <v>49</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>290</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="6">
         <v>50</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>210</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="6">
         <v>52</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>120</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <v>51</v>
       </c>
     </row>
@@ -8360,37 +8461,37 @@
       <c r="E13" s="1">
         <v>3.11</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <v>310</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>62</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <v>310</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="6">
         <v>52</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="6">
         <v>310</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="6">
         <v>56</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="6">
         <v>300</v>
       </c>
-      <c r="S13" s="7">
+      <c r="S13" s="6">
         <v>74</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="6">
         <v>180</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13" s="6">
         <v>74</v>
       </c>
     </row>
@@ -8444,11 +8545,11 @@
       <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="K16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
@@ -8470,10 +8571,10 @@
         <v>15</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
@@ -8492,13 +8593,13 @@
       <c r="F18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="1">
         <v>120</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="1">
         <v>51</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="11">
         <v>2.6880000000000002</v>
       </c>
     </row>
@@ -8524,7 +8625,7 @@
       <c r="L19" s="1">
         <v>53</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
@@ -8548,7 +8649,7 @@
       <c r="L20" s="1">
         <v>56</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
@@ -8569,7 +8670,7 @@
       <c r="L21" s="1">
         <v>62</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
@@ -8593,7 +8694,7 @@
       <c r="L22" s="1">
         <v>64</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
@@ -8611,13 +8712,13 @@
       <c r="F23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="1">
         <v>170</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="1">
         <v>68</v>
       </c>
-      <c r="M23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
@@ -8635,13 +8736,13 @@
       <c r="F24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="5">
         <v>180</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="5">
         <v>74</v>
       </c>
-      <c r="M24" s="6"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
@@ -8661,24 +8762,24 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="K26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L26" s="6"/>
+      <c r="K26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="7"/>
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
       <c r="K27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
@@ -8694,10 +8795,10 @@
       <c r="E28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="1">
         <v>120</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="1">
         <v>51</v>
       </c>
     </row>
@@ -8794,10 +8895,10 @@
       <c r="E33" s="1">
         <v>3.8039999999999998</v>
       </c>
-      <c r="K33" s="12">
+      <c r="K33" s="5">
         <v>180</v>
       </c>
-      <c r="L33" s="12">
+      <c r="L33" s="5">
         <v>74</v>
       </c>
     </row>
@@ -8928,32 +9029,32 @@
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="12">
+      <c r="B43" s="5">
         <v>310</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="5">
         <v>11.65</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="5">
         <v>62</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="5">
         <v>3.7719999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="T10:U10"/>
     <mergeCell ref="L9:U9"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="K16:M16"/>
     <mergeCell ref="M18:M24"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:U10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8962,64 +9063,847 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9C5B90-C6E1-41ED-9691-C41D9E719940}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="9">
+        <v>12.487500000000001</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+      <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6">
+        <v>270</v>
+      </c>
+      <c r="D6" s="6">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6">
+        <v>290</v>
+      </c>
+      <c r="F6" s="6">
+        <v>49</v>
+      </c>
+      <c r="G6" s="6">
+        <v>290</v>
+      </c>
+      <c r="H6" s="6">
+        <v>50</v>
+      </c>
+      <c r="I6" s="6">
+        <v>210</v>
+      </c>
+      <c r="J6" s="6">
+        <v>52</v>
+      </c>
+      <c r="K6" s="6">
         <v>120</v>
       </c>
-      <c r="C3" s="1">
+      <c r="L6" s="6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6">
+        <v>310</v>
+      </c>
+      <c r="D7" s="6">
+        <v>62</v>
+      </c>
+      <c r="E7" s="6">
+        <v>310</v>
+      </c>
+      <c r="F7" s="6">
+        <v>52</v>
+      </c>
+      <c r="G7" s="6">
+        <v>310</v>
+      </c>
+      <c r="H7" s="6">
+        <v>56</v>
+      </c>
+      <c r="I7" s="6">
+        <v>300</v>
+      </c>
+      <c r="J7" s="6">
+        <v>74</v>
+      </c>
+      <c r="K7" s="6">
+        <v>180</v>
+      </c>
+      <c r="L7" s="6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="B10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="K11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="N11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>270</v>
+      </c>
+      <c r="C13" s="1">
         <v>51</v>
       </c>
-      <c r="E3" s="1">
-        <v>2.6829999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E13" s="1">
+        <v>290</v>
+      </c>
+      <c r="F13" s="1">
+        <v>49</v>
+      </c>
+      <c r="H13" s="1">
+        <v>290</v>
+      </c>
+      <c r="I13" s="1">
+        <v>50</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1">
+        <v>50</v>
+      </c>
+      <c r="N13" s="1">
+        <v>120</v>
+      </c>
+      <c r="O13" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
+        <v>55</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
+        <v>55</v>
+      </c>
+      <c r="N14" s="1">
+        <v>135</v>
+      </c>
+      <c r="O14" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
+        <v>310</v>
+      </c>
+      <c r="C15" s="5">
+        <v>62</v>
+      </c>
+      <c r="E15" s="5">
+        <v>310</v>
+      </c>
+      <c r="F15" s="5">
+        <v>52</v>
+      </c>
+      <c r="H15" s="5">
+        <v>310</v>
+      </c>
+      <c r="I15" s="5">
+        <v>56</v>
+      </c>
+      <c r="K15" s="17">
+        <v>310</v>
+      </c>
+      <c r="L15" s="5">
+        <v>56</v>
+      </c>
+      <c r="N15" s="1">
+        <v>145</v>
+      </c>
+      <c r="O15" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="N16" s="1">
+        <v>164</v>
+      </c>
+      <c r="O16" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="N17" s="1">
+        <v>172</v>
+      </c>
+      <c r="O17" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="N18" s="5">
+        <v>180</v>
+      </c>
+      <c r="O18" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="9">
+        <v>11.65</v>
+      </c>
+      <c r="C22" s="6">
+        <v>270</v>
+      </c>
+      <c r="D22" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+      <c r="C23" s="6">
+        <v>290</v>
+      </c>
+      <c r="D23" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="9"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="9"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="9"/>
+      <c r="C26" s="6">
+        <v>310</v>
+      </c>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="9">
+        <v>12.49</v>
+      </c>
+      <c r="C27" s="6">
+        <v>290</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B28" s="9"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="9"/>
+      <c r="C29" s="6">
+        <v>310</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="9">
+        <v>13.33</v>
+      </c>
+      <c r="C30" s="6">
+        <v>290</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="9"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="9"/>
+      <c r="C32" s="6">
+        <v>310</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="9">
+        <v>14.16</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="9"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="9"/>
+      <c r="C35" s="6">
+        <v>310</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="9">
+        <v>15</v>
+      </c>
+      <c r="C36" s="6">
+        <v>120</v>
+      </c>
+      <c r="D36" s="6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="9"/>
+      <c r="C37" s="6">
+        <v>135</v>
+      </c>
+      <c r="D37" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="9"/>
+      <c r="C38" s="6">
+        <v>145</v>
+      </c>
+      <c r="D38" s="6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="9"/>
+      <c r="C39" s="6">
+        <v>164</v>
+      </c>
+      <c r="D39" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="9"/>
+      <c r="C40" s="6">
+        <v>172</v>
+      </c>
+      <c r="D40" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="9"/>
+      <c r="C41" s="6">
+        <v>180</v>
+      </c>
+      <c r="D41" s="6">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B10:O10"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B065C34-D71F-4F02-8C1B-51E36B9B764A}">
+  <dimension ref="B2:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="E5" s="19">
+        <v>41.47</v>
+      </c>
+      <c r="F5" s="19">
+        <v>41.067500000000003</v>
+      </c>
+      <c r="G5" s="19">
+        <v>40.585999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="19">
+        <v>47.106666666666598</v>
+      </c>
+      <c r="F6" s="19">
+        <v>46.8</v>
+      </c>
+      <c r="G6" s="19">
+        <v>46.14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>110</v>
+      </c>
+      <c r="E7" s="19">
+        <v>49.12</v>
+      </c>
+      <c r="F7" s="19">
+        <v>48.015000000000001</v>
+      </c>
+      <c r="G7" s="19">
+        <v>47.59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1">
+        <v>51</v>
+      </c>
+      <c r="E8" s="19">
+        <v>54.349999999999902</v>
+      </c>
+      <c r="F8" s="19">
+        <v>53.445</v>
+      </c>
+      <c r="G8" s="19">
+        <v>52.903999999999897</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>130</v>
+      </c>
+      <c r="E9" s="19">
+        <v>56.77</v>
+      </c>
+      <c r="F9" s="19">
+        <v>56.467500000000001</v>
+      </c>
+      <c r="G9" s="19">
+        <v>55.8019999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>135</v>
+      </c>
+      <c r="C10" s="1">
+        <v>56</v>
+      </c>
+      <c r="E10" s="19">
+        <v>58.779999999999902</v>
+      </c>
+      <c r="F10" s="19">
+        <v>57.9774999999999</v>
+      </c>
+      <c r="G10" s="19">
+        <v>57.491999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>145</v>
+      </c>
+      <c r="C11" s="1">
+        <v>59</v>
+      </c>
+      <c r="E11" s="19">
+        <v>62.003333333333302</v>
+      </c>
+      <c r="F11" s="19">
+        <v>61.295000000000002</v>
+      </c>
+      <c r="G11" s="19">
+        <v>60.631999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="E12" s="19">
+        <v>62.406666666666602</v>
+      </c>
+      <c r="F12" s="19">
+        <v>61.599999999999902</v>
+      </c>
+      <c r="G12" s="19">
+        <v>61.116</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>164</v>
+      </c>
+      <c r="C13" s="1">
+        <v>65</v>
+      </c>
+      <c r="E13" s="19">
+        <v>67.636666666666599</v>
+      </c>
+      <c r="F13" s="19">
+        <v>67.032499999999999</v>
+      </c>
+      <c r="G13" s="19">
+        <v>66.427999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>170</v>
+      </c>
+      <c r="E14" s="19">
+        <v>68.843333333333305</v>
+      </c>
+      <c r="F14" s="19">
+        <v>68.239999999999995</v>
+      </c>
+      <c r="G14" s="19">
+        <v>67.64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>172</v>
+      </c>
+      <c r="C15" s="1">
+        <v>69</v>
+      </c>
+      <c r="E15" s="19">
+        <v>69.653333333333293</v>
+      </c>
+      <c r="F15" s="19">
+        <v>69.144999999999996</v>
+      </c>
+      <c r="G15" s="19">
+        <v>68.603999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>186</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="E16" s="19">
+        <v>74.886666666666599</v>
+      </c>
+      <c r="F16" s="19">
+        <v>74.284999999999997</v>
+      </c>
+      <c r="G16" s="19">
+        <v>74.158000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>190</v>
+      </c>
+      <c r="E17" s="19">
+        <v>74.483333333333306</v>
+      </c>
+      <c r="F17" s="19">
+        <v>73.98</v>
+      </c>
+      <c r="G17" s="19">
+        <v>73.436000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>210</v>
+      </c>
+      <c r="E18" s="19">
+        <v>79.716666666666598</v>
+      </c>
+      <c r="F18" s="19">
+        <v>79.412499999999994</v>
+      </c>
+      <c r="G18" s="19">
+        <v>78.991999999999905</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>230</v>
+      </c>
+      <c r="E19" s="19">
+        <v>84.546666666666596</v>
+      </c>
+      <c r="F19" s="19">
+        <v>84.245000000000005</v>
+      </c>
+      <c r="G19" s="19">
+        <v>83.822000000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>